<commit_message>
refactor: Use "Field Name" to replace "Field ID", and labeling the fields to get their new "Field ID"
</commit_message>
<xml_diff>
--- a/data/land_stats.xlsx
+++ b/data/land_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\zivmax\CUMCM_2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7DA72D-E2BB-41E6-BB36-B6762FE959A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8774A21A-4F92-4789-8875-5C828970D99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38310" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{ADA3BE48-B93D-418F-B554-787C5CA63620}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{ADA3BE48-B93D-418F-B554-787C5CA63620}"/>
   </bookViews>
   <sheets>
     <sheet name="乡村的现有耕地" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>地块编号</t>
+    <t>地块名称</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -609,6 +609,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -617,9 +620,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -940,8 +940,8 @@
   </sheetPr>
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D55"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -954,7 +954,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -977,7 +977,7 @@
       <c r="C2" s="2">
         <v>80</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>59</v>
       </c>
     </row>
@@ -991,7 +991,7 @@
       <c r="C3" s="2">
         <v>55</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1003,7 +1003,7 @@
       <c r="C4" s="2">
         <v>35</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1015,7 +1015,7 @@
       <c r="C5" s="2">
         <v>72</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1027,7 +1027,7 @@
       <c r="C6" s="3">
         <v>68</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -1039,7 +1039,7 @@
       <c r="C7" s="2">
         <v>55</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -1051,7 +1051,7 @@
       <c r="C8" s="2">
         <v>60</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1063,7 +1063,7 @@
       <c r="C9" s="2">
         <v>46</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1075,7 +1075,7 @@
       <c r="C10" s="2">
         <v>40</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1087,7 +1087,7 @@
       <c r="C11" s="2">
         <v>28</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -1099,7 +1099,7 @@
       <c r="C12" s="2">
         <v>25</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -1111,7 +1111,7 @@
       <c r="C13" s="2">
         <v>86</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1123,7 +1123,7 @@
       <c r="C14" s="2">
         <v>55</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -1135,7 +1135,7 @@
       <c r="C15" s="2">
         <v>44</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -1147,7 +1147,7 @@
       <c r="C16" s="2">
         <v>50</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -1159,7 +1159,7 @@
       <c r="C17" s="2">
         <v>25</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -1171,7 +1171,7 @@
       <c r="C18" s="2">
         <v>60</v>
       </c>
-      <c r="D18" s="7"/>
+      <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -1183,7 +1183,7 @@
       <c r="C19" s="2">
         <v>45</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="8"/>
     </row>
     <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -1195,7 +1195,7 @@
       <c r="C20" s="2">
         <v>35</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -1207,7 +1207,7 @@
       <c r="C21" s="2">
         <v>20</v>
       </c>
-      <c r="D21" s="7"/>
+      <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
@@ -1219,7 +1219,7 @@
       <c r="C22" s="2">
         <v>15</v>
       </c>
-      <c r="D22" s="7"/>
+      <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -1231,7 +1231,7 @@
       <c r="C23" s="2">
         <v>13</v>
       </c>
-      <c r="D23" s="7"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -1243,7 +1243,7 @@
       <c r="C24" s="2">
         <v>15</v>
       </c>
-      <c r="D24" s="7"/>
+      <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -1255,7 +1255,7 @@
       <c r="C25" s="2">
         <v>18</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -1267,7 +1267,7 @@
       <c r="C26" s="2">
         <v>27</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="D26" s="8"/>
     </row>
     <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -1279,7 +1279,7 @@
       <c r="C27" s="2">
         <v>20</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
@@ -1291,7 +1291,7 @@
       <c r="C28" s="2">
         <v>15</v>
       </c>
-      <c r="D28" s="7"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -1303,7 +1303,7 @@
       <c r="C29" s="2">
         <v>10</v>
       </c>
-      <c r="D29" s="7"/>
+      <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
@@ -1315,7 +1315,7 @@
       <c r="C30" s="2">
         <v>14</v>
       </c>
-      <c r="D30" s="7"/>
+      <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
@@ -1327,7 +1327,7 @@
       <c r="C31" s="2">
         <v>6</v>
       </c>
-      <c r="D31" s="7"/>
+      <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
@@ -1339,7 +1339,7 @@
       <c r="C32" s="2">
         <v>10</v>
       </c>
-      <c r="D32" s="7"/>
+      <c r="D32" s="8"/>
     </row>
     <row r="33" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -1351,7 +1351,7 @@
       <c r="C33" s="2">
         <v>12</v>
       </c>
-      <c r="D33" s="7"/>
+      <c r="D33" s="8"/>
     </row>
     <row r="34" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
@@ -1363,7 +1363,7 @@
       <c r="C34" s="2">
         <v>22</v>
       </c>
-      <c r="D34" s="7"/>
+      <c r="D34" s="8"/>
     </row>
     <row r="35" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
@@ -1375,7 +1375,7 @@
       <c r="C35" s="2">
         <v>20</v>
       </c>
-      <c r="D35" s="7"/>
+      <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
@@ -1387,7 +1387,7 @@
       <c r="C36" s="2">
         <v>0.6</v>
       </c>
-      <c r="D36" s="7"/>
+      <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -1399,7 +1399,7 @@
       <c r="C37" s="2">
         <v>0.6</v>
       </c>
-      <c r="D37" s="7"/>
+      <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
@@ -1411,7 +1411,7 @@
       <c r="C38" s="2">
         <v>0.6</v>
       </c>
-      <c r="D38" s="7"/>
+      <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -1423,7 +1423,7 @@
       <c r="C39" s="2">
         <v>0.6</v>
       </c>
-      <c r="D39" s="7"/>
+      <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -1435,7 +1435,7 @@
       <c r="C40" s="2">
         <v>0.6</v>
       </c>
-      <c r="D40" s="7"/>
+      <c r="D40" s="8"/>
     </row>
     <row r="41" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
@@ -1447,7 +1447,7 @@
       <c r="C41" s="2">
         <v>0.6</v>
       </c>
-      <c r="D41" s="7"/>
+      <c r="D41" s="8"/>
     </row>
     <row r="42" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
@@ -1459,7 +1459,7 @@
       <c r="C42" s="2">
         <v>0.6</v>
       </c>
-      <c r="D42" s="7"/>
+      <c r="D42" s="8"/>
     </row>
     <row r="43" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
@@ -1471,7 +1471,7 @@
       <c r="C43" s="2">
         <v>0.6</v>
       </c>
-      <c r="D43" s="7"/>
+      <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
@@ -1483,7 +1483,7 @@
       <c r="C44" s="2">
         <v>0.6</v>
       </c>
-      <c r="D44" s="7"/>
+      <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
@@ -1495,7 +1495,7 @@
       <c r="C45" s="2">
         <v>0.6</v>
       </c>
-      <c r="D45" s="7"/>
+      <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
@@ -1507,7 +1507,7 @@
       <c r="C46" s="2">
         <v>0.6</v>
       </c>
-      <c r="D46" s="7"/>
+      <c r="D46" s="8"/>
     </row>
     <row r="47" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
@@ -1519,7 +1519,7 @@
       <c r="C47" s="2">
         <v>0.6</v>
       </c>
-      <c r="D47" s="7"/>
+      <c r="D47" s="8"/>
     </row>
     <row r="48" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
@@ -1531,7 +1531,7 @@
       <c r="C48" s="2">
         <v>0.6</v>
       </c>
-      <c r="D48" s="7"/>
+      <c r="D48" s="8"/>
     </row>
     <row r="49" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
@@ -1543,7 +1543,7 @@
       <c r="C49" s="2">
         <v>0.6</v>
       </c>
-      <c r="D49" s="7"/>
+      <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
@@ -1555,7 +1555,7 @@
       <c r="C50" s="2">
         <v>0.6</v>
       </c>
-      <c r="D50" s="7"/>
+      <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
@@ -1567,7 +1567,7 @@
       <c r="C51" s="2">
         <v>0.6</v>
       </c>
-      <c r="D51" s="7"/>
+      <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
@@ -1579,7 +1579,7 @@
       <c r="C52" s="2">
         <v>0.6</v>
       </c>
-      <c r="D52" s="7"/>
+      <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
@@ -1591,7 +1591,7 @@
       <c r="C53" s="2">
         <v>0.6</v>
       </c>
-      <c r="D53" s="7"/>
+      <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
@@ -1603,7 +1603,7 @@
       <c r="C54" s="2">
         <v>0.6</v>
       </c>
-      <c r="D54" s="7"/>
+      <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
@@ -1615,7 +1615,7 @@
       <c r="C55" s="2">
         <v>0.6</v>
       </c>
-      <c r="D55" s="8"/>
+      <c r="D55" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>